<commit_message>
create json using json lib
</commit_message>
<xml_diff>
--- a/python/DataSets/rezh_geo.xlsx
+++ b/python/DataSets/rezh_geo.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="355">
   <si>
     <t>ADRESS</t>
   </si>
@@ -893,6 +893,9 @@
   </si>
   <si>
     <t>Nonbank credit organization "MOBI. Money" Limited Liability Company NCO "MOBI. Money" LLC</t>
+  </si>
+  <si>
+    <t>ООО НКО "Расчетные Решения»</t>
   </si>
   <si>
     <t>область Свердловская, городской округ Режевской, город Реж, улица Машиностроителей, д 3</t>
@@ -1117,7 +1120,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1132,13 +1135,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -1165,28 +1168,28 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1195,28 +1198,28 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1233,7 +1236,7 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1242,28 +1245,28 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1283,8 +1286,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1435,9 +1438,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1517,7 +1520,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1545,10 +1548,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1804,9 +1807,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -2094,7 +2097,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2122,10 +2125,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2382,7 +2385,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="8" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85156" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5625" style="1" customWidth="1"/>
+    <col min="5" max="8" width="8.85156" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5217,7 +5223,9 @@
       <c r="B115" t="s" s="8">
         <v>175</v>
       </c>
-      <c r="C115" s="10"/>
+      <c r="C115" t="s" s="9">
+        <v>293</v>
+      </c>
       <c r="D115" t="s" s="9">
         <v>281</v>
       </c>
@@ -5237,7 +5245,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s" s="8">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C116" t="s" s="9">
         <v>280</v>
@@ -5250,10 +5258,10 @@
       </c>
       <c r="F116" s="10"/>
       <c r="G116" t="s" s="9">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="H116" t="s" s="9">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="117" ht="13.55" customHeight="1">
@@ -5261,10 +5269,10 @@
         <v>115</v>
       </c>
       <c r="B117" t="s" s="8">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C117" t="s" s="9">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D117" t="s" s="9">
         <v>281</v>
@@ -5274,10 +5282,10 @@
       </c>
       <c r="F117" s="10"/>
       <c r="G117" t="s" s="9">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H117" t="s" s="9">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="118" ht="13.55" customHeight="1">
@@ -5285,10 +5293,10 @@
         <v>116</v>
       </c>
       <c r="B118" t="s" s="8">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C118" t="s" s="9">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D118" t="s" s="9">
         <v>281</v>
@@ -5309,10 +5317,10 @@
         <v>117</v>
       </c>
       <c r="B119" t="s" s="8">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C119" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D119" t="s" s="9">
         <v>281</v>
@@ -5321,7 +5329,7 @@
         <v>282</v>
       </c>
       <c r="F119" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G119" t="s" s="9">
         <v>114</v>
@@ -5335,10 +5343,10 @@
         <v>118</v>
       </c>
       <c r="B120" t="s" s="8">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C120" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D120" t="s" s="9">
         <v>281</v>
@@ -5347,7 +5355,7 @@
         <v>282</v>
       </c>
       <c r="F120" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G120" t="s" s="9">
         <v>240</v>
@@ -5361,10 +5369,10 @@
         <v>119</v>
       </c>
       <c r="B121" t="s" s="8">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C121" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D121" t="s" s="9">
         <v>281</v>
@@ -5373,7 +5381,7 @@
         <v>282</v>
       </c>
       <c r="F121" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G121" t="s" s="9">
         <v>237</v>
@@ -5387,10 +5395,10 @@
         <v>120</v>
       </c>
       <c r="B122" t="s" s="8">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C122" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D122" t="s" s="9">
         <v>281</v>
@@ -5399,7 +5407,7 @@
         <v>282</v>
       </c>
       <c r="F122" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G122" t="s" s="9">
         <v>234</v>
@@ -5413,10 +5421,10 @@
         <v>121</v>
       </c>
       <c r="B123" t="s" s="8">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C123" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D123" t="s" s="9">
         <v>281</v>
@@ -5425,7 +5433,7 @@
         <v>282</v>
       </c>
       <c r="F123" t="s" s="9">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G123" t="s" s="9">
         <v>177</v>
@@ -5439,10 +5447,10 @@
         <v>122</v>
       </c>
       <c r="B124" t="s" s="8">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C124" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D124" t="s" s="9">
         <v>281</v>
@@ -5451,7 +5459,7 @@
         <v>282</v>
       </c>
       <c r="F124" t="s" s="9">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G124" t="s" s="9">
         <v>65</v>
@@ -5465,10 +5473,10 @@
         <v>123</v>
       </c>
       <c r="B125" t="s" s="8">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C125" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D125" t="s" s="9">
         <v>281</v>
@@ -5477,13 +5485,13 @@
         <v>282</v>
       </c>
       <c r="F125" t="s" s="9">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G125" t="s" s="9">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H125" t="s" s="9">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="126" ht="13.55" customHeight="1">
@@ -5491,10 +5499,10 @@
         <v>124</v>
       </c>
       <c r="B126" t="s" s="8">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C126" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D126" t="s" s="9">
         <v>281</v>
@@ -5503,7 +5511,7 @@
         <v>282</v>
       </c>
       <c r="F126" t="s" s="9">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="G126" t="s" s="9">
         <v>75</v>
@@ -5517,10 +5525,10 @@
         <v>125</v>
       </c>
       <c r="B127" t="s" s="8">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C127" t="s" s="9">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D127" t="s" s="9">
         <v>281</v>
@@ -5541,10 +5549,10 @@
         <v>126</v>
       </c>
       <c r="B128" t="s" s="8">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C128" t="s" s="9">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D128" t="s" s="9">
         <v>281</v>
@@ -5567,10 +5575,10 @@
         <v>127</v>
       </c>
       <c r="B129" t="s" s="8">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C129" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D129" t="s" s="9">
         <v>281</v>
@@ -5579,7 +5587,7 @@
         <v>282</v>
       </c>
       <c r="F129" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G129" t="s" s="9">
         <v>243</v>
@@ -5593,10 +5601,10 @@
         <v>128</v>
       </c>
       <c r="B130" t="s" s="8">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C130" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D130" t="s" s="9">
         <v>281</v>
@@ -5605,7 +5613,7 @@
         <v>282</v>
       </c>
       <c r="F130" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G130" t="s" s="9">
         <v>246</v>
@@ -5619,10 +5627,10 @@
         <v>129</v>
       </c>
       <c r="B131" t="s" s="8">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C131" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D131" t="s" s="9">
         <v>281</v>
@@ -5631,7 +5639,7 @@
         <v>282</v>
       </c>
       <c r="F131" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G131" t="s" s="9">
         <v>249</v>
@@ -5645,10 +5653,10 @@
         <v>130</v>
       </c>
       <c r="B132" t="s" s="8">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C132" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D132" t="s" s="9">
         <v>281</v>
@@ -5657,7 +5665,7 @@
         <v>282</v>
       </c>
       <c r="F132" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G132" t="s" s="9">
         <v>252</v>
@@ -5671,10 +5679,10 @@
         <v>131</v>
       </c>
       <c r="B133" t="s" s="8">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C133" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D133" t="s" s="9">
         <v>281</v>
@@ -5683,13 +5691,13 @@
         <v>282</v>
       </c>
       <c r="F133" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G133" t="s" s="9">
         <v>255</v>
       </c>
       <c r="H133" t="s" s="9">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="134" ht="13.55" customHeight="1">
@@ -5697,10 +5705,10 @@
         <v>132</v>
       </c>
       <c r="B134" t="s" s="8">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C134" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D134" t="s" s="9">
         <v>281</v>
@@ -5709,7 +5717,7 @@
         <v>282</v>
       </c>
       <c r="F134" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G134" t="s" s="9">
         <v>257</v>
@@ -5723,10 +5731,10 @@
         <v>133</v>
       </c>
       <c r="B135" t="s" s="8">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C135" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D135" t="s" s="9">
         <v>281</v>
@@ -5735,7 +5743,7 @@
         <v>282</v>
       </c>
       <c r="F135" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G135" t="s" s="9">
         <v>260</v>
@@ -5749,10 +5757,10 @@
         <v>134</v>
       </c>
       <c r="B136" t="s" s="8">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C136" t="s" s="9">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D136" t="s" s="9">
         <v>281</v>
@@ -5761,7 +5769,7 @@
         <v>282</v>
       </c>
       <c r="F136" t="s" s="9">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G136" t="s" s="9">
         <v>263</v>
@@ -5775,23 +5783,23 @@
         <v>135</v>
       </c>
       <c r="B137" t="s" s="8">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C137" t="s" s="9">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D137" t="s" s="9">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E137" t="s" s="9">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F137" s="10"/>
       <c r="G137" t="s" s="9">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H137" t="s" s="9">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="138" ht="13.55" customHeight="1">
@@ -5799,23 +5807,23 @@
         <v>136</v>
       </c>
       <c r="B138" t="s" s="8">
+        <v>331</v>
+      </c>
+      <c r="C138" t="s" s="9">
+        <v>332</v>
+      </c>
+      <c r="D138" t="s" s="9">
+        <v>329</v>
+      </c>
+      <c r="E138" t="s" s="9">
         <v>330</v>
-      </c>
-      <c r="C138" t="s" s="9">
-        <v>331</v>
-      </c>
-      <c r="D138" t="s" s="9">
-        <v>328</v>
-      </c>
-      <c r="E138" t="s" s="9">
-        <v>329</v>
       </c>
       <c r="F138" s="10"/>
       <c r="G138" t="s" s="9">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="H138" t="s" s="9">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="139" ht="13.55" customHeight="1">
@@ -5823,16 +5831,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="s" s="8">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C139" t="s" s="9">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D139" t="s" s="9">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E139" t="s" s="9">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F139" s="10"/>
       <c r="G139" t="s" s="9">
@@ -5847,16 +5855,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="s" s="8">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C140" t="s" s="9">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D140" t="s" s="9">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E140" t="s" s="9">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F140" s="10"/>
       <c r="G140" t="s" s="9">
@@ -5871,23 +5879,23 @@
         <v>139</v>
       </c>
       <c r="B141" t="s" s="8">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C141" t="s" s="9">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D141" t="s" s="9">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E141" t="s" s="9">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F141" s="10"/>
       <c r="G141" t="s" s="9">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="H141" t="s" s="9">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="142" ht="13.55" customHeight="1">
@@ -5895,16 +5903,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="s" s="8">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C142" t="s" s="9">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D142" t="s" s="9">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E142" t="s" s="9">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F142" s="10"/>
       <c r="G142" t="s" s="9">
@@ -5919,16 +5927,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="s" s="8">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C143" t="s" s="9">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D143" t="s" s="9">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E143" t="s" s="9">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F143" s="10"/>
       <c r="G143" t="s" s="9">
@@ -5943,16 +5951,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="s" s="8">
+        <v>345</v>
+      </c>
+      <c r="C144" t="s" s="9">
+        <v>346</v>
+      </c>
+      <c r="D144" t="s" s="9">
+        <v>343</v>
+      </c>
+      <c r="E144" t="s" s="9">
         <v>344</v>
-      </c>
-      <c r="C144" t="s" s="9">
-        <v>345</v>
-      </c>
-      <c r="D144" t="s" s="9">
-        <v>342</v>
-      </c>
-      <c r="E144" t="s" s="9">
-        <v>343</v>
       </c>
       <c r="F144" s="10"/>
       <c r="G144" t="s" s="9">
@@ -5967,23 +5975,23 @@
         <v>143</v>
       </c>
       <c r="B145" t="s" s="8">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C145" t="s" s="9">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="D145" t="s" s="9">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E145" t="s" s="9">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F145" s="10"/>
       <c r="G145" t="s" s="9">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H145" t="s" s="9">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="146" ht="13.55" customHeight="1">
@@ -5991,23 +5999,23 @@
         <v>144</v>
       </c>
       <c r="B146" t="s" s="8">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C146" t="s" s="9">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D146" t="s" s="9">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E146" t="s" s="9">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="F146" s="10"/>
       <c r="G146" t="s" s="9">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="H146" t="s" s="9">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>